<commit_message>
Update formulas and table format
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/8_Date_and_Time_Functions.xlsx
+++ b/2_Formulas_Functions/8_Date_and_Time_Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB41794D-3AC3-41AE-99A3-90AA9FFED7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0691AA28-5E8C-46A7-8DCF-FF1EFBEB8762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6" yWindow="384" windowWidth="18132" windowHeight="11478" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36720" yWindow="2685" windowWidth="18330" windowHeight="12855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="8" r:id="rId1"/>
@@ -786,19 +786,19 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.26953125" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -824,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -850,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -876,7 +876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -902,7 +902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -928,7 +928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -954,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -980,7 +980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -1357,26 +1357,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3969B28-4CA1-4CA9-A455-FC26EC1A58EA}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>

</xml_diff>